<commit_message>
cleaned crime logs for ohio university
</commit_message>
<xml_diff>
--- a/Data/campus_daily_crime_log/crime_log_list.xlsx
+++ b/Data/campus_daily_crime_log/crime_log_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/campus_daily_crime_log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3393750D-0D78-B442-BE62-AA198DDA8CD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A278E670-6E05-1445-855C-71ECE609CD10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{E56BBE90-010A-6847-B84D-6F70C739D039}"/>
   </bookViews>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7000A663-FA10-6A4E-8552-26224935F959}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1323,16 +1323,19 @@
         <v>1</v>
       </c>
       <c r="D22" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>107</v>
       </c>
       <c r="F22" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="6">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1915,15 +1918,15 @@
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F46">
         <f>SUM(F2:F45)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G46">
         <f>SUM(G2:G45)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small changes to logs
</commit_message>
<xml_diff>
--- a/Data/campus_daily_crime_log/crime_log_list.xlsx
+++ b/Data/campus_daily_crime_log/crime_log_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/campus_daily_crime_log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A278E670-6E05-1445-855C-71ECE609CD10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749641F7-3467-B640-954F-EE6D50EECC35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{E56BBE90-010A-6847-B84D-6F70C739D039}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{E56BBE90-010A-6847-B84D-6F70C739D039}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="116">
   <si>
     <t>University</t>
   </si>
@@ -369,6 +369,21 @@
   </si>
   <si>
     <t>not confident about how to collapse this one because of missing case numbers and missing other info</t>
+  </si>
+  <si>
+    <t>Texas Christian University</t>
+  </si>
+  <si>
+    <t>Hampden-Sydney College</t>
+  </si>
+  <si>
+    <t>University of Kentucky</t>
+  </si>
+  <si>
+    <t>University of Nebraska-Lincoln</t>
+  </si>
+  <si>
+    <t>University of Nevada-Reno</t>
   </si>
 </sst>
 </file>
@@ -775,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7000A663-FA10-6A4E-8552-26224935F959}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -1939,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527FB6C9-1533-1049-8024-A75763BC480C}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2420,6 +2435,15 @@
       <c r="A22" t="s">
         <v>98</v>
       </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
       <c r="F22">
         <v>0</v>
       </c>
@@ -2881,6 +2905,106 @@
         <v>0</v>
       </c>
       <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to literature review
</commit_message>
<xml_diff>
--- a/Data/campus_daily_crime_log/crime_log_list.xlsx
+++ b/Data/campus_daily_crime_log/crime_log_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/campus_daily_crime_log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A3945B-17DB-DE4F-9F3D-AF04A411EC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ECB358-08A2-A746-AF57-4189AB78B955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="2520" windowWidth="35840" windowHeight="21100" activeTab="1" xr2:uid="{E56BBE90-010A-6847-B84D-6F70C739D039}"/>
   </bookViews>
@@ -2022,8 +2022,8 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P21" sqref="P21"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
hope this one works
</commit_message>
<xml_diff>
--- a/Data/campus_daily_crime_log/crime_log_list.xlsx
+++ b/Data/campus_daily_crime_log/crime_log_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/campus_daily_crime_log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21AC0C2-61EF-E140-A2F6-51CC59188519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097D1C6B-EA30-0148-93BC-F0B9D6BA4EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1300" windowWidth="35840" windowHeight="21100" activeTab="1" xr2:uid="{E56BBE90-010A-6847-B84D-6F70C739D039}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21100" activeTab="1" xr2:uid="{E56BBE90-010A-6847-B84D-6F70C739D039}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="154">
   <si>
     <t>University</t>
   </si>
@@ -441,6 +441,63 @@
   </si>
   <si>
     <t>Syracuse University</t>
+  </si>
+  <si>
+    <t>Albany State University</t>
+  </si>
+  <si>
+    <t>California State University-Chico</t>
+  </si>
+  <si>
+    <t>DePauw University</t>
+  </si>
+  <si>
+    <t>James Madison University</t>
+  </si>
+  <si>
+    <t>Michigan State University</t>
+  </si>
+  <si>
+    <t>North Carolina Central University</t>
+  </si>
+  <si>
+    <t>Prairie View A &amp; M University</t>
+  </si>
+  <si>
+    <t>Southern Methodist University</t>
+  </si>
+  <si>
+    <t>University of Arizona</t>
+  </si>
+  <si>
+    <t>The University of Texas at Arlington</t>
+  </si>
+  <si>
+    <t>University of Arkansas</t>
+  </si>
+  <si>
+    <t>University of California-Santa Barbara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Delaware </t>
+  </si>
+  <si>
+    <t>University of Mississippi</t>
+  </si>
+  <si>
+    <t>University of Wisconsin-Madison</t>
+  </si>
+  <si>
+    <t>no 2014</t>
+  </si>
+  <si>
+    <t>only 2017-2019</t>
+  </si>
+  <si>
+    <t>no december 2018 or all 2019</t>
+  </si>
+  <si>
+    <t>University of Illinois at Urbana-Champaign</t>
   </si>
 </sst>
 </file>
@@ -2025,11 +2082,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527FB6C9-1533-1049-8024-A75763BC480C}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2073,13 +2130,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2088,21 +2145,21 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2120,6 +2177,9 @@
         <v>0</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
@@ -2128,13 +2188,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2143,7 +2203,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2156,17 +2216,20 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2183,7 +2246,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2211,11 +2274,17 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>73</v>
+      <c r="A7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2231,43 +2300,43 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>125</v>
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>93</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -2280,43 +2349,46 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
+      <c r="A10" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>130</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>119</v>
+      <c r="A11" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -2327,13 +2399,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2342,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -2356,14 +2428,11 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
       <c r="D13">
         <v>1</v>
       </c>
@@ -2371,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -2384,26 +2453,17 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
+      <c r="A14" t="s">
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2414,11 +2474,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
       <c r="D15">
         <v>1</v>
       </c>
@@ -2439,14 +2502,14 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
+      <c r="A16" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2455,7 +2518,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -2469,7 +2532,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2498,14 +2561,11 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
-        <v>43</v>
-      </c>
       <c r="D18">
         <v>1</v>
       </c>
@@ -2526,14 +2586,14 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
+      <c r="A19" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2542,7 +2602,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2555,14 +2615,14 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
+      <c r="A20" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2571,27 +2631,27 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2600,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2613,14 +2673,20 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>18</v>
+      <c r="A22" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>91</v>
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2637,19 +2703,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2665,12 +2731,15 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>133</v>
+      <c r="A24" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
       <c r="D24">
         <v>1</v>
       </c>
@@ -2691,14 +2760,20 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>20</v>
+      <c r="A25" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2715,13 +2790,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2730,10 +2805,10 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2744,13 +2819,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2772,20 +2847,14 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>23</v>
+      <c r="A28" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2801,8 +2870,20 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>116</v>
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -2819,10 +2900,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2835,8 +2925,14 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
-        <v>122</v>
+      <c r="A31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -2852,11 +2948,14 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>111</v>
+      <c r="A32" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="B32">
         <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2879,13 +2978,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2894,10 +2993,10 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -2907,11 +3006,23 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
-        <v>117</v>
+      <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -2924,11 +3035,20 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
-        <v>127</v>
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>43</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2945,13 +3065,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2960,7 +3080,7 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2973,20 +3093,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
+      <c r="A37" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -3002,14 +3110,11 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" t="s">
-        <v>74</v>
+      <c r="A38" t="s">
+        <v>134</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3023,7 +3128,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -3039,8 +3144,17 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="13" t="s">
-        <v>123</v>
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -3056,8 +3170,20 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
-        <v>124</v>
+      <c r="A41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -3073,20 +3199,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
+      <c r="A42" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -3102,20 +3216,11 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
+      <c r="A43" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -3131,43 +3236,28 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
+      <c r="A44" s="13" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3180,12 +3270,15 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>113</v>
+      <c r="A46" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
       <c r="D46">
         <v>1</v>
       </c>
@@ -3206,8 +3299,20 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
-        <v>120</v>
+      <c r="A47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -3223,14 +3328,20 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>31</v>
+      <c r="A48" t="s">
+        <v>49</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>43</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -3247,19 +3358,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -3275,17 +3377,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>114</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
+      <c r="A50" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -3301,17 +3394,8 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>115</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
+      <c r="A51" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -3327,11 +3411,20 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>33</v>
+      <c r="A52" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>152</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -3347,20 +3440,8 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>43</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
+      <c r="A53" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -3376,8 +3457,20 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="13" t="s">
-        <v>118</v>
+      <c r="A54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -3393,8 +3486,20 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="13" t="s">
-        <v>121</v>
+      <c r="A55" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -3410,8 +3515,20 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>51</v>
+      <c r="A56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -3427,14 +3544,14 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>50</v>
+      <c r="A57" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3446,7 +3563,7 @@
         <v>1</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -3457,7 +3574,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -3486,56 +3603,433 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C75" t="s">
         <v>75</v>
       </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>43</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I60">
-    <sortCondition ref="A2:A60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I76">
+    <sortCondition ref="A3:A76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>